<commit_message>
Update QR generation URL and data files
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="128">
   <si>
     <t>user_id</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>admin@library.com</t>
+  </si>
+  <si>
+    <t>3324968856</t>
   </si>
   <si>
     <t>ADMIN</t>
@@ -786,7 +789,7 @@
         <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -797,7 +800,7 @@
         <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -808,7 +811,7 @@
         <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -819,7 +822,7 @@
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -829,8 +832,11 @@
       <c r="B6" t="s">
         <v>70</v>
       </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
       <c r="E6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -841,7 +847,7 @@
         <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -852,7 +858,7 @@
         <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -863,7 +869,7 @@
         <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -874,7 +880,7 @@
         <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -885,7 +891,7 @@
         <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -896,7 +902,7 @@
         <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -907,7 +913,7 @@
         <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -918,7 +924,7 @@
         <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -929,7 +935,7 @@
         <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -940,7 +946,7 @@
         <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -951,7 +957,7 @@
         <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -962,7 +968,7 @@
         <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -973,7 +979,7 @@
         <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -984,7 +990,7 @@
         <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -995,7 +1001,7 @@
         <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1006,7 +1012,7 @@
         <v>85</v>
       </c>
       <c r="E22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1017,7 +1023,7 @@
         <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1028,7 +1034,7 @@
         <v>87</v>
       </c>
       <c r="E24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1039,7 +1045,7 @@
         <v>88</v>
       </c>
       <c r="E25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1050,7 +1056,7 @@
         <v>89</v>
       </c>
       <c r="E26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1061,7 +1067,7 @@
         <v>90</v>
       </c>
       <c r="E27" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1072,7 +1078,7 @@
         <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1083,7 +1089,7 @@
         <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1094,7 +1100,7 @@
         <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1105,7 +1111,7 @@
         <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1116,7 +1122,7 @@
         <v>95</v>
       </c>
       <c r="E32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1127,7 +1133,7 @@
         <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1138,7 +1144,7 @@
         <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1149,7 +1155,7 @@
         <v>98</v>
       </c>
       <c r="E35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1160,7 +1166,7 @@
         <v>99</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1171,7 +1177,7 @@
         <v>100</v>
       </c>
       <c r="E37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1182,7 +1188,7 @@
         <v>101</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1193,7 +1199,7 @@
         <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1204,7 +1210,7 @@
         <v>103</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1215,7 +1221,7 @@
         <v>104</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1226,7 +1232,7 @@
         <v>105</v>
       </c>
       <c r="E42" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1237,7 +1243,7 @@
         <v>98</v>
       </c>
       <c r="E43" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1248,7 +1254,7 @@
         <v>106</v>
       </c>
       <c r="E44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1259,7 +1265,7 @@
         <v>107</v>
       </c>
       <c r="E45" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1270,7 +1276,7 @@
         <v>108</v>
       </c>
       <c r="E46" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1281,7 +1287,7 @@
         <v>109</v>
       </c>
       <c r="E47" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1292,7 +1298,7 @@
         <v>110</v>
       </c>
       <c r="E48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1303,7 +1309,7 @@
         <v>111</v>
       </c>
       <c r="E49" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1314,7 +1320,7 @@
         <v>112</v>
       </c>
       <c r="E50" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1325,7 +1331,7 @@
         <v>113</v>
       </c>
       <c r="E51" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1336,7 +1342,7 @@
         <v>114</v>
       </c>
       <c r="E52" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1347,7 +1353,7 @@
         <v>83</v>
       </c>
       <c r="E53" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1358,7 +1364,7 @@
         <v>115</v>
       </c>
       <c r="E54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1369,7 +1375,7 @@
         <v>116</v>
       </c>
       <c r="E55" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1380,7 +1386,7 @@
         <v>117</v>
       </c>
       <c r="E56" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1391,7 +1397,7 @@
         <v>118</v>
       </c>
       <c r="E57" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1402,7 +1408,7 @@
         <v>119</v>
       </c>
       <c r="E58" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1413,7 +1419,7 @@
         <v>120</v>
       </c>
       <c r="E59" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1424,7 +1430,7 @@
         <v>121</v>
       </c>
       <c r="E60" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1435,7 +1441,7 @@
         <v>122</v>
       </c>
       <c r="E61" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1446,7 +1452,7 @@
         <v>123</v>
       </c>
       <c r="E62" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Enhanced Library App (Lend/Return flow, Auto-Renumbering, Admin Delete/Edit, Inline Mobile Update)
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
   <si>
     <t>user_id</t>
   </si>
@@ -184,214 +184,157 @@
     <t>MEM-051</t>
   </si>
   <si>
-    <t>MEM-052</t>
-  </si>
-  <si>
-    <t>MEM-053</t>
-  </si>
-  <si>
-    <t>MEM-054</t>
-  </si>
-  <si>
-    <t>MEM-055</t>
-  </si>
-  <si>
-    <t>MEM-056</t>
-  </si>
-  <si>
-    <t>MEM-057</t>
-  </si>
-  <si>
-    <t>MEM-058</t>
-  </si>
-  <si>
-    <t>MEM-059</t>
-  </si>
-  <si>
-    <t>MEM-060</t>
-  </si>
-  <si>
-    <t>MEM-061</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>Ganesh</t>
-  </si>
-  <si>
-    <t>Aadhithiyan Kalivarthan</t>
-  </si>
-  <si>
-    <t>Sundaravel</t>
+    <t>Sri</t>
+  </si>
+  <si>
+    <t>Ganeshan</t>
+  </si>
+  <si>
+    <t>Senthil</t>
+  </si>
+  <si>
+    <t>muthu kumaresan</t>
+  </si>
+  <si>
+    <t>Queretaro</t>
+  </si>
+  <si>
+    <t>Kalai Priya</t>
+  </si>
+  <si>
+    <t>Magesh (tamil class)</t>
   </si>
   <si>
     <t>Anand</t>
   </si>
   <si>
-    <t>Kishore Kumar</t>
-  </si>
-  <si>
-    <t>Senthil</t>
-  </si>
-  <si>
-    <t>muthu kumaresan</t>
+    <t>Gangesh</t>
+  </si>
+  <si>
+    <t>Surya</t>
+  </si>
+  <si>
+    <t>Selva</t>
+  </si>
+  <si>
+    <t>Babu</t>
+  </si>
+  <si>
+    <t>Shake</t>
+  </si>
+  <si>
+    <t>Shanmugapriyan</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>Saidai Jagan</t>
+  </si>
+  <si>
+    <t>benazir (tamil class)</t>
+  </si>
+  <si>
+    <t>Muthusamy</t>
+  </si>
+  <si>
+    <t>Sasikumar</t>
+  </si>
+  <si>
+    <t>Maheswari</t>
+  </si>
+  <si>
+    <t>Chandra prakash</t>
+  </si>
+  <si>
+    <t>Naveen</t>
+  </si>
+  <si>
+    <t>Muruganantham</t>
+  </si>
+  <si>
+    <t>Vignesh (AI)</t>
+  </si>
+  <si>
+    <t>Hariprasad</t>
+  </si>
+  <si>
+    <t>Arun Bharani</t>
+  </si>
+  <si>
+    <t>Suganya</t>
+  </si>
+  <si>
+    <t>Priyanka sathish</t>
+  </si>
+  <si>
+    <t>Susidevi</t>
+  </si>
+  <si>
+    <t>Kasirajan</t>
+  </si>
+  <si>
+    <t>varatharaj</t>
   </si>
   <si>
     <t>Hari Prakash</t>
   </si>
   <si>
-    <t>Queretaro</t>
-  </si>
-  <si>
-    <t>Kalai Priya</t>
-  </si>
-  <si>
-    <t>Puru</t>
-  </si>
-  <si>
-    <t>Surya</t>
-  </si>
-  <si>
-    <t>Selva</t>
-  </si>
-  <si>
-    <t>Shake</t>
+    <t>Logeshwari</t>
+  </si>
+  <si>
+    <t>Stela</t>
+  </si>
+  <si>
+    <t>Mahesh</t>
+  </si>
+  <si>
+    <t>SuryaDevi</t>
+  </si>
+  <si>
+    <t>Vignesh</t>
+  </si>
+  <si>
+    <t>sibi</t>
+  </si>
+  <si>
+    <t>hariprasad</t>
+  </si>
+  <si>
+    <t>Anbuvel</t>
+  </si>
+  <si>
+    <t>Thoufik</t>
   </si>
   <si>
     <t>Divya</t>
   </si>
   <si>
-    <t>Hari</t>
-  </si>
-  <si>
-    <t>Saidai Jagan</t>
-  </si>
-  <si>
-    <t>Balaji Natarajan</t>
-  </si>
-  <si>
-    <t>Arun Bharani</t>
-  </si>
-  <si>
-    <t>Quretaro</t>
-  </si>
-  <si>
-    <t>Maheswari</t>
-  </si>
-  <si>
-    <t>Chandra prakash</t>
-  </si>
-  <si>
-    <t>Aravind</t>
-  </si>
-  <si>
-    <t>Sri</t>
-  </si>
-  <si>
-    <t>Naveen</t>
-  </si>
-  <si>
-    <t>sibi</t>
-  </si>
-  <si>
-    <t>Muruganantham</t>
-  </si>
-  <si>
-    <t>Suganya</t>
-  </si>
-  <si>
-    <t>Gomathi</t>
-  </si>
-  <si>
-    <t>Queretari</t>
-  </si>
-  <si>
-    <t>Prabha selvaraj</t>
-  </si>
-  <si>
-    <t>Logeshwari</t>
-  </si>
-  <si>
-    <t>Stela</t>
-  </si>
-  <si>
-    <t>Lavanya</t>
-  </si>
-  <si>
-    <t>Mahesh</t>
-  </si>
-  <si>
-    <t>SuryaDevi</t>
-  </si>
-  <si>
-    <t>Vignesh</t>
-  </si>
-  <si>
-    <t>Thompson</t>
-  </si>
-  <si>
-    <t>Anbuvel</t>
-  </si>
-  <si>
-    <t>Thoufik</t>
-  </si>
-  <si>
-    <t>cibi</t>
-  </si>
-  <si>
-    <t>Aadhi</t>
-  </si>
-  <si>
-    <t>Quertero</t>
-  </si>
-  <si>
     <t>Rajeswari</t>
   </si>
   <si>
-    <t>Muthusamy</t>
-  </si>
-  <si>
     <t>Indrasenan</t>
   </si>
   <si>
-    <t>Ganeshan</t>
-  </si>
-  <si>
-    <t>Gangesh</t>
-  </si>
-  <si>
-    <t>Karthik</t>
-  </si>
-  <si>
-    <t>Babu</t>
-  </si>
-  <si>
-    <t>Balaji</t>
-  </si>
-  <si>
-    <t>sampath</t>
-  </si>
-  <si>
-    <t>Prakash Karthikeyan</t>
-  </si>
-  <si>
-    <t>Baskar Murugeshan</t>
-  </si>
-  <si>
-    <t>Kasirajan</t>
-  </si>
-  <si>
-    <t>shanmuga priyan</t>
-  </si>
-  <si>
-    <t>muthu</t>
+    <t>sri</t>
+  </si>
+  <si>
+    <t>banupriya</t>
+  </si>
+  <si>
+    <t>Ragavan</t>
+  </si>
+  <si>
+    <t>Vignesh V</t>
   </si>
   <si>
     <t>admin@library.com</t>
   </si>
   <si>
-    <t>3324968856</t>
+    <t>vignesh29498@gmail.com</t>
   </si>
   <si>
     <t>ADMIN</t>
@@ -755,7 +698,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -783,13 +726,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -797,10 +740,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -808,10 +751,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -819,10 +762,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -830,13 +773,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -844,10 +784,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -855,10 +795,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -866,10 +806,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -877,10 +817,10 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -888,10 +828,10 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -899,10 +839,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -910,10 +850,10 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -921,10 +861,10 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -932,10 +872,10 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -943,10 +883,10 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -954,10 +894,10 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -965,10 +905,10 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -976,10 +916,10 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -987,10 +927,10 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1001,7 +941,7 @@
         <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1009,10 +949,10 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1020,10 +960,10 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1031,10 +971,10 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1042,10 +982,10 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1053,10 +993,10 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1064,10 +1004,10 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1075,10 +1015,10 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1086,10 +1026,10 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E29" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1097,10 +1037,10 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1108,10 +1048,10 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E31" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1119,10 +1059,10 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E32" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1130,10 +1070,10 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E33" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1141,10 +1081,10 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1152,10 +1092,10 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1163,10 +1103,10 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E36" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1174,10 +1114,10 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E37" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1185,10 +1125,10 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1196,10 +1136,10 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E39" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1207,10 +1147,10 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E40" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1218,10 +1158,10 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E41" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1229,10 +1169,10 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1240,10 +1180,10 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E43" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1251,10 +1191,10 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E44" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1262,10 +1202,10 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E45" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1273,10 +1213,10 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E46" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1284,10 +1224,10 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E47" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1295,10 +1235,10 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E48" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1306,10 +1246,10 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E49" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1317,10 +1257,10 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E50" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1328,10 +1268,10 @@
         <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E51" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1339,120 +1279,16 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
+        <v>104</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52">
+        <v>9080314434</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" t="s">
-        <v>115</v>
-      </c>
-      <c r="E54" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" t="s">
-        <v>116</v>
-      </c>
-      <c r="E55" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" t="s">
-        <v>117</v>
-      </c>
-      <c r="E56" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" t="s">
-        <v>118</v>
-      </c>
-      <c r="E57" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" t="s">
-        <v>119</v>
-      </c>
-      <c r="E58" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" t="s">
-        <v>120</v>
-      </c>
-      <c r="E59" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>63</v>
-      </c>
-      <c r="B60" t="s">
-        <v>121</v>
-      </c>
-      <c r="E60" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" t="s">
-        <v>122</v>
-      </c>
-      <c r="E61" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" t="s">
-        <v>123</v>
-      </c>
-      <c r="E62" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>